<commit_message>
Update template email bulk excel
</commit_message>
<xml_diff>
--- a/downloads/email_deac_bulk.xlsx
+++ b/downloads/email_deac_bulk.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PortalPilot\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D4C9E9-A989-46AE-879D-A439F634A223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D85823C-C2CD-45A4-AD66-D4C560EFBF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{445FB331-9226-4A81-BC99-47DF256F7C61}"/>
   </bookViews>
@@ -401,7 +401,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,34 +412,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change data type in excel from general to text
</commit_message>
<xml_diff>
--- a/downloads/email_deac_bulk.xlsx
+++ b/downloads/email_deac_bulk.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PortalPilot\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D85823C-C2CD-45A4-AD66-D4C560EFBF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A95873D-5602-4282-905D-2A4FA94E2B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{445FB331-9226-4A81-BC99-47DF256F7C61}"/>
   </bookViews>
@@ -81,9 +81,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,44 +402,45 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change template of account number to format 1234***5678
</commit_message>
<xml_diff>
--- a/downloads/email_deac_bulk.xlsx
+++ b/downloads/email_deac_bulk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PortalPilot\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A95873D-5602-4282-905D-2A4FA94E2B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4E47E7-D365-4098-87B0-C88481FD4E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{445FB331-9226-4A81-BC99-47DF256F7C61}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>016601020870555</t>
   </si>
   <si>
-    <t>1660XXXXXXXX758</t>
-  </si>
-  <si>
     <t>email address</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>abdul@gmail.com</t>
+  </si>
+  <si>
+    <t>1660***5758</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +414,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -422,15 +422,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -438,7 +438,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>

</xml_diff>